<commit_message>
another change to pin table ig
also add temp file to git ignore
</commit_message>
<xml_diff>
--- a/Pins/Organized_Pin_Table.xlsx
+++ b/Pins/Organized_Pin_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kin\mechatronics-goats\Pins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyrum/Documents/Arduino/mechatronics-goats/Pins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499DDE1E-0CBB-40DE-9642-8A0FC98343AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AEDF9B-E3F5-794F-BB4F-527D7B75AE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-6855" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21600" yWindow="11600" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usages" sheetId="1" r:id="rId1"/>
@@ -504,7 +504,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,6 +558,24 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -609,7 +627,7 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -626,6 +644,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
@@ -957,20 +978,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="164" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -981,7 +1002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -991,8 +1012,10 @@
       <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="12"/>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1002,8 +1025,10 @@
       <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="12"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1013,8 +1038,10 @@
       <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="12"/>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1022,8 +1049,9 @@
         <v>10</v>
       </c>
       <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1031,8 +1059,9 @@
         <v>12</v>
       </c>
       <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -1042,8 +1071,9 @@
       <c r="C7" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -1053,8 +1083,9 @@
       <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
@@ -1064,8 +1095,10 @@
       <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -1075,8 +1108,10 @@
       <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -1086,8 +1121,10 @@
       <c r="C11" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
@@ -1095,8 +1132,9 @@
         <v>10</v>
       </c>
       <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -1104,8 +1142,9 @@
         <v>12</v>
       </c>
       <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1115,8 +1154,9 @@
       <c r="C14" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
@@ -1126,8 +1166,9 @@
       <c r="C15" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
@@ -1138,7 +1179,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>26</v>
       </c>
@@ -1149,7 +1190,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>26</v>
       </c>
@@ -1160,7 +1201,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
@@ -1169,7 +1210,7 @@
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
@@ -1178,7 +1219,7 @@
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
@@ -1189,7 +1230,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -1200,7 +1241,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>34</v>
       </c>
@@ -1211,7 +1252,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>34</v>
       </c>
@@ -1222,7 +1263,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>34</v>
       </c>
@@ -1233,7 +1274,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>34</v>
       </c>
@@ -1242,7 +1283,7 @@
       </c>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>34</v>
       </c>
@@ -1251,7 +1292,7 @@
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>34</v>
       </c>
@@ -1262,7 +1303,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>34</v>
       </c>
@@ -1273,7 +1314,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>42</v>
       </c>
@@ -1284,7 +1325,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>42</v>
       </c>
@@ -1295,7 +1336,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>42</v>
       </c>
@@ -1306,7 +1347,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>42</v>
       </c>
@@ -1317,7 +1358,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>42</v>
       </c>
@@ -1328,7 +1369,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
@@ -1339,7 +1380,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>47</v>
       </c>
@@ -1350,7 +1391,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>47</v>
       </c>
@@ -1361,7 +1402,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>50</v>
       </c>
@@ -1372,7 +1413,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>50</v>
       </c>
@@ -1383,7 +1424,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>51</v>
       </c>
@@ -1392,7 +1433,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>53</v>
       </c>
@@ -1401,7 +1442,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>55</v>
       </c>
@@ -1410,7 +1451,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>55</v>
       </c>
@@ -1419,7 +1460,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>55</v>
       </c>
@@ -1428,7 +1469,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>55</v>
       </c>
@@ -1437,7 +1478,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>55</v>
       </c>
@@ -1446,7 +1487,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
         <v>55</v>
       </c>
@@ -1455,7 +1496,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>55</v>
       </c>
@@ -1464,7 +1505,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>63</v>
       </c>
@@ -1473,7 +1514,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
         <v>63</v>
       </c>
@@ -1482,7 +1523,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>67</v>
       </c>
@@ -1493,7 +1534,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
         <v>67</v>
       </c>
@@ -1504,7 +1545,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
         <v>67</v>
       </c>
@@ -1515,7 +1556,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
         <v>67</v>
       </c>
@@ -1526,12 +1567,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>139</v>
       </c>
@@ -1540,7 +1581,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
         <v>139</v>
       </c>
@@ -1558,16 +1599,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" workbookViewId="0">
+    <sheetView showRowColHeaders="0" topLeftCell="A4" zoomScale="150" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>68</v>
       </c>
@@ -1581,7 +1622,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1596,7 +1637,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -1611,7 +1652,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1626,7 +1667,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -1641,7 +1682,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -1656,7 +1697,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -1671,7 +1712,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -1686,7 +1727,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -1701,7 +1742,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1716,7 +1757,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1731,7 +1772,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1746,7 +1787,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -1761,7 +1802,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1776,7 +1817,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -1791,7 +1832,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -1806,7 +1847,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -1821,7 +1862,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -1836,7 +1877,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -1851,7 +1892,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -1866,7 +1907,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -1881,7 +1922,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -1896,7 +1937,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -1911,7 +1952,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -1926,7 +1967,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -1941,7 +1982,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -1956,7 +1997,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -1971,7 +2012,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>72</v>
       </c>
@@ -1986,7 +2027,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -2001,7 +2042,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>72</v>
       </c>
@@ -2016,7 +2057,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -2031,7 +2072,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -2046,7 +2087,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -2061,7 +2102,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -2076,7 +2117,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -2091,7 +2132,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -2106,7 +2147,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2121,7 +2162,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -2136,7 +2177,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -2151,7 +2192,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -2166,7 +2207,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -2181,7 +2222,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -2196,7 +2237,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -2211,7 +2252,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -2226,7 +2267,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -2241,7 +2282,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>72</v>
       </c>
@@ -2256,7 +2297,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -2271,7 +2312,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -2286,7 +2327,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -2301,7 +2342,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>72</v>
       </c>
@@ -2316,7 +2357,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>72</v>
       </c>
@@ -2331,7 +2372,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>72</v>
       </c>
@@ -2346,7 +2387,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>72</v>
       </c>
@@ -2361,7 +2402,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>72</v>
       </c>
@@ -2376,7 +2417,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -2391,7 +2432,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -2406,7 +2447,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -2421,7 +2462,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>88</v>
       </c>
@@ -2436,7 +2477,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>88</v>
       </c>
@@ -2451,7 +2492,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>88</v>
       </c>
@@ -2466,7 +2507,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -2481,7 +2522,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>88</v>
       </c>
@@ -2496,7 +2537,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>88</v>
       </c>
@@ -2511,7 +2552,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>88</v>
       </c>
@@ -2526,7 +2567,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>88</v>
       </c>
@@ -2541,7 +2582,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>88</v>
       </c>
@@ -2556,7 +2597,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>88</v>
       </c>
@@ -2571,7 +2612,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>88</v>
       </c>
@@ -2586,7 +2627,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>88</v>
       </c>
@@ -2601,7 +2642,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>88</v>
       </c>
@@ -2616,7 +2657,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Add 99 bogus pins to diagnostic and current monitoring
</commit_message>
<xml_diff>
--- a/Pins/Organized_Pin_Table.xlsx
+++ b/Pins/Organized_Pin_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyrum/Documents/Arduino/mechatronics-goats/Pins/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kinblandford/Documents/Arduino/mechatronics-goats/Pins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AEDF9B-E3F5-794F-BB4F-527D7B75AE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAD14AB-8339-D34A-9616-52530F6F63BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21600" yWindow="11600" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usages" sheetId="1" r:id="rId1"/>
@@ -504,7 +504,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -576,6 +576,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -627,7 +633,7 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -647,6 +653,8 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
@@ -980,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="164" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1048,7 +1056,9 @@
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="16">
+        <v>99</v>
+      </c>
       <c r="E5" s="14"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1058,7 +1068,9 @@
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="16">
+        <v>99</v>
+      </c>
       <c r="E6" s="14"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1131,7 +1143,9 @@
       <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="15">
+        <v>99</v>
+      </c>
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1141,7 +1155,9 @@
       <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="15">
+        <v>99</v>
+      </c>
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1208,7 +1224,9 @@
       <c r="B19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="15">
+        <v>99</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
@@ -1217,7 +1235,9 @@
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="15">
+        <v>99</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
@@ -1281,7 +1301,9 @@
       <c r="B26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="15">
+        <v>99</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
@@ -1290,7 +1312,9 @@
       <c r="B27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="15">
+        <v>99</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">

</xml_diff>

<commit_message>
Update pintable -- A9 for CM conflicts
</commit_message>
<xml_diff>
--- a/Pins/Organized_Pin_Table.xlsx
+++ b/Pins/Organized_Pin_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kinblandford/Documents/Arduino/mechatronics-goats/Pins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAD14AB-8339-D34A-9616-52530F6F63BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514731EB-6AE3-8648-88F0-EA0D974E91E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="140">
   <si>
     <t>Hardware Device</t>
   </si>
@@ -989,7 +989,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1068,8 +1068,8 @@
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="16">
-        <v>99</v>
+      <c r="C6" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="E6" s="14"/>
     </row>
@@ -1155,8 +1155,8 @@
       <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="15">
-        <v>99</v>
+      <c r="C13" s="15" t="s">
+        <v>92</v>
       </c>
       <c r="E13" s="13"/>
     </row>
@@ -1235,8 +1235,8 @@
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="15">
-        <v>99</v>
+      <c r="C20" s="15" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1312,8 +1312,8 @@
       <c r="B27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="15">
-        <v>99</v>
+      <c r="C27" s="15" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2603,7 +2603,7 @@
       </c>
       <c r="D65" t="str">
         <f>IF(ISNUMBER(MATCH("A9", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Free</v>
+        <v>Used</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add missing pin and add empty IR example
</commit_message>
<xml_diff>
--- a/Pins/Organized_Pin_Table.xlsx
+++ b/Pins/Organized_Pin_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kinblandford/Documents/Arduino/mechatronics-goats/Pins/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kin\mechatronics-goats\Pins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514731EB-6AE3-8648-88F0-EA0D974E91E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854B2872-E30D-4927-A06B-1C44F0C28AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-6855" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usages" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="140">
   <si>
     <t>Hardware Device</t>
   </si>
@@ -986,20 +986,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="164" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1023,7 +1023,7 @@
       <c r="D2" s="12"/>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1036,7 +1036,7 @@
       <c r="D3" s="12"/>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1049,7 +1049,7 @@
       <c r="D4" s="12"/>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1073,7 +1073,7 @@
       </c>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="E7" s="14"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
@@ -1110,7 +1110,7 @@
       <c r="D9" s="12"/>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -1123,7 +1123,7 @@
       <c r="D10" s="12"/>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -1136,7 +1136,7 @@
       <c r="D11" s="12"/>
       <c r="E11" s="13"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="E12" s="13"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="E13" s="13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="E14" s="13"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="E15" s="13"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>26</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>26</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>34</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>34</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>34</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>34</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>34</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>34</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>34</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>42</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>42</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>42</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>42</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>42</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>47</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>47</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>50</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>50</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>51</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>53</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>55</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>55</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>55</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>55</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>55</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>55</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>55</v>
       </c>
@@ -1529,88 +1529,97 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>67</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>67</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>67</v>
       </c>
       <c r="B54" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C55" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>139</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1623,16 +1632,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" topLeftCell="A4" zoomScale="150" workbookViewId="0">
+    <sheetView showRowColHeaders="0" topLeftCell="A16" zoomScale="150" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>68</v>
       </c>
@@ -1646,7 +1655,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1661,7 +1670,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -1676,7 +1685,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1691,7 +1700,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -1706,7 +1715,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -1721,7 +1730,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -1736,7 +1745,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -1751,7 +1760,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -1766,7 +1775,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1781,7 +1790,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1796,7 +1805,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1811,7 +1820,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -1826,7 +1835,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1841,7 +1850,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -1856,7 +1865,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -1871,7 +1880,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -1886,7 +1895,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -1901,7 +1910,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -1916,7 +1925,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -1931,7 +1940,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -1946,7 +1955,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -1961,7 +1970,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -1976,7 +1985,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -1991,7 +2000,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -2006,7 +2015,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -2021,7 +2030,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2036,7 +2045,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>72</v>
       </c>
@@ -2051,7 +2060,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -2066,7 +2075,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>72</v>
       </c>
@@ -2081,7 +2090,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -2096,7 +2105,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -2111,7 +2120,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -2126,7 +2135,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -2141,7 +2150,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -2156,7 +2165,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -2171,7 +2180,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2186,7 +2195,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -2201,7 +2210,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -2216,7 +2225,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -2231,7 +2240,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -2246,7 +2255,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -2261,7 +2270,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -2276,7 +2285,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -2291,7 +2300,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -2303,10 +2312,10 @@
       </c>
       <c r="D45" t="str">
         <f>IF(ISNUMBER(MATCH("D43", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Free</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>Used</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>72</v>
       </c>
@@ -2321,7 +2330,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -2336,7 +2345,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -2351,7 +2360,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -2366,7 +2375,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>72</v>
       </c>
@@ -2381,7 +2390,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>72</v>
       </c>
@@ -2396,7 +2405,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>72</v>
       </c>
@@ -2411,7 +2420,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>72</v>
       </c>
@@ -2426,7 +2435,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>72</v>
       </c>
@@ -2441,7 +2450,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -2456,7 +2465,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -2471,7 +2480,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -2486,7 +2495,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>88</v>
       </c>
@@ -2501,7 +2510,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>88</v>
       </c>
@@ -2516,7 +2525,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>88</v>
       </c>
@@ -2531,7 +2540,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -2546,7 +2555,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>88</v>
       </c>
@@ -2561,7 +2570,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>88</v>
       </c>
@@ -2576,7 +2585,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>88</v>
       </c>
@@ -2591,7 +2600,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>88</v>
       </c>
@@ -2606,7 +2615,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>88</v>
       </c>
@@ -2621,7 +2630,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>88</v>
       </c>
@@ -2636,7 +2645,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>88</v>
       </c>
@@ -2651,7 +2660,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>88</v>
       </c>
@@ -2666,7 +2675,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>88</v>
       </c>
@@ -2681,7 +2690,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Update pin table to add TV remote pin
</commit_message>
<xml_diff>
--- a/Pins/Organized_Pin_Table.xlsx
+++ b/Pins/Organized_Pin_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kin\mechatronics-goats\Pins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kinblandford/Documents/Arduino/mechatronics-goats/Pins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854B2872-E30D-4927-A06B-1C44F0C28AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06415313-BB0F-7C4D-9319-A68E08B185C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-6855" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usages" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="142">
   <si>
     <t>Hardware Device</t>
   </si>
@@ -454,6 +454,12 @@
   </si>
   <si>
     <t>Arduino Reserved</t>
+  </si>
+  <si>
+    <t>IR Remote</t>
+  </si>
+  <si>
+    <t>Decode</t>
   </si>
 </sst>
 </file>
@@ -484,13 +490,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -503,8 +502,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -582,6 +588,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -622,16 +633,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -641,22 +653,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="8"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="9"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
     <cellStyle name="40% - Accent3" xfId="4" builtinId="39"/>
     <cellStyle name="40% - Accent4" xfId="5" builtinId="43"/>
@@ -665,6 +677,7 @@
     <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
     <cellStyle name="60% - Accent4" xfId="6" builtinId="44"/>
     <cellStyle name="Accent2" xfId="2" builtinId="33"/>
+    <cellStyle name="Accent3" xfId="9" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -988,18 +1001,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="164" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="164" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1010,616 +1023,622 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="14"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <v>99</v>
       </c>
-      <c r="E5" s="14"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="14"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="14"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="14"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>99</v>
       </c>
-      <c r="E12" s="13"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="13"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="13"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="13"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="14">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="14">
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7" t="s">
+      <c r="B40" s="6"/>
+      <c r="C40" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7" t="s">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10" t="s">
+      <c r="B42" s="9"/>
+      <c r="C42" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10" t="s">
+      <c r="B43" s="9"/>
+      <c r="C43" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10" t="s">
+      <c r="B44" s="9"/>
+      <c r="C44" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10" t="s">
+      <c r="B45" s="9"/>
+      <c r="C45" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10" t="s">
+      <c r="B46" s="9"/>
+      <c r="C46" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10" t="s">
+      <c r="B47" s="9"/>
+      <c r="C47" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10" t="s">
+      <c r="B48" s="9"/>
+      <c r="C48" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10" t="s">
+      <c r="B49" s="9"/>
+      <c r="C49" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8" t="s">
+      <c r="B50" s="7"/>
+      <c r="C50" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8" t="s">
+      <c r="B51" s="7"/>
+      <c r="C51" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C53" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
+    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11" t="s">
+      <c r="B57" s="10"/>
+      <c r="C57" s="10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11" t="s">
+      <c r="B58" s="10"/>
+      <c r="C58" s="10" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1632,16 +1651,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" topLeftCell="A16" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showRowColHeaders="0" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>68</v>
       </c>
@@ -1655,7 +1674,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1670,7 +1689,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -1685,7 +1704,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1700,7 +1719,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -1715,7 +1734,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -1730,7 +1749,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -1745,7 +1764,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -1760,7 +1779,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -1775,7 +1794,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1790,7 +1809,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1805,7 +1824,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1820,7 +1839,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -1832,10 +1851,10 @@
       </c>
       <c r="D13" t="str">
         <f>IF(ISNUMBER(MATCH("D11", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Free</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>Used</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1850,7 +1869,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -1865,7 +1884,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -1880,7 +1899,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -1895,7 +1914,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -1910,7 +1929,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -1925,7 +1944,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -1940,7 +1959,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -1955,7 +1974,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -1970,7 +1989,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -1985,7 +2004,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -2000,7 +2019,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -2015,7 +2034,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -2030,7 +2049,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2045,7 +2064,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>72</v>
       </c>
@@ -2060,7 +2079,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -2075,7 +2094,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>72</v>
       </c>
@@ -2090,7 +2109,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -2105,7 +2124,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -2120,7 +2139,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -2135,7 +2154,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -2150,7 +2169,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -2165,7 +2184,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -2180,7 +2199,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2195,7 +2214,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -2210,7 +2229,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -2225,7 +2244,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -2240,7 +2259,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -2255,7 +2274,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -2270,7 +2289,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -2285,7 +2304,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -2300,7 +2319,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -2315,7 +2334,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>72</v>
       </c>
@@ -2330,7 +2349,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -2345,7 +2364,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -2360,7 +2379,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -2375,7 +2394,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>72</v>
       </c>
@@ -2390,7 +2409,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>72</v>
       </c>
@@ -2405,7 +2424,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>72</v>
       </c>
@@ -2420,7 +2439,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>72</v>
       </c>
@@ -2435,7 +2454,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>72</v>
       </c>
@@ -2450,7 +2469,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -2465,7 +2484,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -2480,7 +2499,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -2495,7 +2514,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>88</v>
       </c>
@@ -2510,7 +2529,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>88</v>
       </c>
@@ -2525,7 +2544,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>88</v>
       </c>
@@ -2540,7 +2559,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -2555,7 +2574,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>88</v>
       </c>
@@ -2570,7 +2589,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>88</v>
       </c>
@@ -2585,7 +2604,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>88</v>
       </c>
@@ -2600,7 +2619,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>88</v>
       </c>
@@ -2615,7 +2634,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>88</v>
       </c>
@@ -2630,7 +2649,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>88</v>
       </c>
@@ -2645,7 +2664,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>88</v>
       </c>
@@ -2660,7 +2679,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>88</v>
       </c>
@@ -2675,7 +2694,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>88</v>
       </c>
@@ -2690,7 +2709,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Update pin table and wiring diagram for color sensor change. SCL and SDA are on D20 and D21. Thus, wheel M1EN has been moved to D12.
</commit_message>
<xml_diff>
--- a/Pins/Organized_Pin_Table.xlsx
+++ b/Pins/Organized_Pin_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kinblandford/Documents/Arduino/mechatronics-goats/Pins/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kin\mechatronics-goats\Pins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06415313-BB0F-7C4D-9319-A68E08B185C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BCB11A-5A4F-4ECA-B17E-09B05CF41A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-6855" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usages" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="140">
   <si>
     <t>Hardware Device</t>
   </si>
@@ -333,18 +333,6 @@
     <t>A15</t>
   </si>
   <si>
-    <t>?1</t>
-  </si>
-  <si>
-    <t>?2</t>
-  </si>
-  <si>
-    <t>?3</t>
-  </si>
-  <si>
-    <t>?4</t>
-  </si>
-  <si>
     <t>TX2</t>
   </si>
   <si>
@@ -460,6 +448,12 @@
   </si>
   <si>
     <t>Decode</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>SCL</t>
   </si>
 </sst>
 </file>
@@ -999,20 +993,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="164" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1036,7 +1030,7 @@
       <c r="D2" s="11"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1049,7 +1043,7 @@
       <c r="D3" s="11"/>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1062,7 +1056,7 @@
       <c r="D4" s="11"/>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1074,7 +1068,7 @@
       </c>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1086,7 +1080,7 @@
       </c>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -1098,7 +1092,7 @@
       </c>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1110,7 +1104,7 @@
       </c>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -1123,7 +1117,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -1136,7 +1130,7 @@
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -1149,7 +1143,7 @@
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1161,7 +1155,7 @@
       </c>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1173,7 +1167,7 @@
       </c>
       <c r="E13" s="12"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
@@ -1181,11 +1175,11 @@
         <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -1197,7 +1191,7 @@
       </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -1208,7 +1202,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
@@ -1219,7 +1213,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>26</v>
       </c>
@@ -1230,7 +1224,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
@@ -1241,7 +1235,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
@@ -1252,7 +1246,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
@@ -1260,10 +1254,10 @@
         <v>14</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
@@ -1274,7 +1268,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>34</v>
       </c>
@@ -1285,7 +1279,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>34</v>
       </c>
@@ -1296,7 +1290,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>34</v>
       </c>
@@ -1307,7 +1301,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
@@ -1318,7 +1312,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>34</v>
       </c>
@@ -1329,7 +1323,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>34</v>
       </c>
@@ -1340,7 +1334,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>34</v>
       </c>
@@ -1351,40 +1345,40 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
@@ -1395,7 +1389,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
@@ -1406,62 +1400,62 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>51</v>
       </c>
@@ -1470,7 +1464,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>53</v>
       </c>
@@ -1479,7 +1473,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>55</v>
       </c>
@@ -1488,7 +1482,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>55</v>
       </c>
@@ -1497,7 +1491,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>55</v>
       </c>
@@ -1506,7 +1500,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>55</v>
       </c>
@@ -1515,7 +1509,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>55</v>
       </c>
@@ -1524,7 +1518,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>55</v>
       </c>
@@ -1533,7 +1527,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>55</v>
       </c>
@@ -1542,7 +1536,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>55</v>
       </c>
@@ -1551,7 +1545,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>63</v>
       </c>
@@ -1560,7 +1554,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>63</v>
       </c>
@@ -1569,76 +1563,54 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B56" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="C56" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1651,16 +1623,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" workbookViewId="0">
+    <sheetView showRowColHeaders="0" topLeftCell="A31" zoomScale="150" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>68</v>
       </c>
@@ -1674,12 +1646,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
         <v>73</v>
@@ -1689,12 +1661,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
         <v>74</v>
@@ -1704,12 +1676,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1719,12 +1691,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -1734,12 +1706,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -1749,12 +1721,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
         <v>43</v>
@@ -1764,12 +1736,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1779,12 +1751,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -1794,12 +1766,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -1809,12 +1781,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -1824,12 +1796,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
@@ -1839,12 +1811,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C13" t="s">
         <v>48</v>
@@ -1854,12 +1826,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
@@ -1869,12 +1841,12 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
         <v>75</v>
@@ -1884,12 +1856,12 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C16" t="s">
         <v>76</v>
@@ -1899,12 +1871,12 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C17" t="s">
         <v>77</v>
@@ -1914,12 +1886,12 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
         <v>78</v>
@@ -1929,12 +1901,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C19" t="s">
         <v>79</v>
@@ -1944,12 +1916,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C20" t="s">
         <v>45</v>
@@ -1959,12 +1931,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
         <v>40</v>
@@ -1974,12 +1946,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
@@ -1989,12 +1961,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C23" t="s">
         <v>24</v>
@@ -2004,7 +1976,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -2019,7 +1991,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -2034,7 +2006,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -2049,7 +2021,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2064,7 +2036,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>72</v>
       </c>
@@ -2079,7 +2051,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -2094,7 +2066,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>72</v>
       </c>
@@ -2109,7 +2081,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -2124,7 +2096,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -2139,7 +2111,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -2154,7 +2126,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -2169,7 +2141,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -2184,7 +2156,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -2199,7 +2171,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2214,7 +2186,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -2229,7 +2201,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -2244,7 +2216,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -2259,7 +2231,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -2274,7 +2246,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -2289,7 +2261,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -2304,7 +2276,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -2319,7 +2291,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -2334,12 +2306,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>72</v>
       </c>
       <c r="B46" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C46" t="s">
         <v>81</v>
@@ -2349,12 +2321,12 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C47" t="s">
         <v>29</v>
@@ -2364,12 +2336,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>72</v>
       </c>
       <c r="B48" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C48" t="s">
         <v>37</v>
@@ -2379,7 +2351,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -2391,10 +2363,10 @@
       </c>
       <c r="D49" t="str">
         <f>IF(ISNUMBER(MATCH("D47", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Used</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>Free</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>72</v>
       </c>
@@ -2409,7 +2381,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>72</v>
       </c>
@@ -2421,10 +2393,10 @@
       </c>
       <c r="D51" t="str">
         <f>IF(ISNUMBER(MATCH("D49", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Used</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>Free</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>72</v>
       </c>
@@ -2439,7 +2411,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>72</v>
       </c>
@@ -2451,10 +2423,10 @@
       </c>
       <c r="D53" t="str">
         <f>IF(ISNUMBER(MATCH("D51", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Used</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>Free</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>72</v>
       </c>
@@ -2469,7 +2441,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -2484,7 +2456,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -2499,7 +2471,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -2514,7 +2486,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>88</v>
       </c>
@@ -2529,7 +2501,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>88</v>
       </c>
@@ -2544,7 +2516,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>88</v>
       </c>
@@ -2559,7 +2531,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -2574,7 +2546,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>88</v>
       </c>
@@ -2586,10 +2558,10 @@
       </c>
       <c r="D62" t="str">
         <f>IF(ISNUMBER(MATCH("A6", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Used</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+        <v>Free</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>88</v>
       </c>
@@ -2604,12 +2576,12 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C64" t="s">
         <v>91</v>
@@ -2619,12 +2591,12 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>88</v>
       </c>
       <c r="B65" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C65" t="s">
         <v>92</v>
@@ -2634,12 +2606,12 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>88</v>
       </c>
       <c r="B66" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C66" t="s">
         <v>93</v>
@@ -2649,12 +2621,12 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>88</v>
       </c>
       <c r="B67" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C67" t="s">
         <v>94</v>
@@ -2664,12 +2636,12 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>88</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C68" t="s">
         <v>95</v>
@@ -2679,12 +2651,12 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>88</v>
       </c>
       <c r="B69" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C69" t="s">
         <v>96</v>
@@ -2694,12 +2666,12 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>88</v>
       </c>
       <c r="B70" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C70" t="s">
         <v>97</v>
@@ -2709,12 +2681,12 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>88</v>
       </c>
       <c r="B71" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C71" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
Update pintable and library for remapping. YOU MUST MAKE THE LIBRARY CHANGE LOCALLY TOO.
</commit_message>
<xml_diff>
--- a/Pins/Organized_Pin_Table.xlsx
+++ b/Pins/Organized_Pin_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kin\mechatronics-goats\Pins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kinblandford/Documents/Arduino/mechatronics-goats/Pins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BCB11A-5A4F-4ECA-B17E-09B05CF41A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B2B6DD-997D-A24F-91A1-1EDAFB7A5856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-6855" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usages" sheetId="1" r:id="rId1"/>
@@ -996,17 +996,17 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1025,12 +1025,12 @@
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1043,7 +1043,7 @@
       <c r="D3" s="11"/>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1056,7 +1056,7 @@
       <c r="D4" s="11"/>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -1117,7 +1117,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -1130,7 +1130,7 @@
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -1143,7 +1143,7 @@
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="E13" s="12"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>26</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>34</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>34</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>34</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>34</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>34</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>34</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>42</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>42</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>42</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>42</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>47</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>47</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>50</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>50</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>51</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>53</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>55</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>55</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>55</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>55</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>55</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>55</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>55</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>55</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>63</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>63</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>67</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>67</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="16" t="s">
         <v>136</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
         <v>135</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
         <v>135</v>
       </c>
@@ -1623,16 +1623,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" topLeftCell="A31" zoomScale="150" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="150" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>68</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1838,10 +1838,10 @@
       </c>
       <c r="D14" t="str">
         <f>IF(ISNUMBER(MATCH("D12", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Free</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>Used</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>72</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>72</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>72</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>72</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>72</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>72</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>72</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>72</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>88</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>88</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>88</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>88</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>88</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>88</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>88</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>Used</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>88</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>88</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>88</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>88</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>88</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>Free</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Add hall to pin table
</commit_message>
<xml_diff>
--- a/Pins/Organized_Pin_Table.xlsx
+++ b/Pins/Organized_Pin_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kinblandford/Documents/Arduino/mechatronics-goats/Pins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B2B6DD-997D-A24F-91A1-1EDAFB7A5856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65202AE2-0572-0E45-9605-6FF9073D3CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="141">
   <si>
     <t>Hardware Device</t>
   </si>
@@ -454,6 +454,9 @@
   </si>
   <si>
     <t>SCL</t>
+  </si>
+  <si>
+    <t>Hall Sensor</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -587,6 +590,12 @@
         <fgColor theme="6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -639,7 +648,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -661,6 +670,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
@@ -993,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1025,7 +1035,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="13"/>
@@ -1564,14 +1574,12 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>32</v>
+      <c r="A52" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1579,30 +1587,32 @@
         <v>67</v>
       </c>
       <c r="B53" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C54" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="16" t="s">
+    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B55" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="C55" s="16" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1611,6 +1621,15 @@
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1623,7 +1642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" workbookViewId="0">
+    <sheetView showRowColHeaders="0" topLeftCell="A47" zoomScale="150" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1838,7 +1857,7 @@
       </c>
       <c r="D14" t="str">
         <f>IF(ISNUMBER(MATCH("D12", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Used</v>
+        <v>Free</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2513,7 +2532,7 @@
       </c>
       <c r="D59" t="str">
         <f>IF(ISNUMBER(MATCH("A3", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Free</v>
+        <v>Used</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Reloading code should be almost done. Just need to implement squareUpUsingProx(), centerOnIrArray(), pushButton().
Needs to be tested, obviously. Currently, most thresholds are guesses, and comparisons may be flipped (because hall effect voltage may be lower in the presence of a field?)
</commit_message>
<xml_diff>
--- a/Pins/Organized_Pin_Table.xlsx
+++ b/Pins/Organized_Pin_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kinblandford/Documents/Arduino/mechatronics-goats/Pins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B2B6DD-997D-A24F-91A1-1EDAFB7A5856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2C7092-4F28-FA44-9DAB-BA2F31ABB277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="141">
   <si>
     <t>Hardware Device</t>
   </si>
@@ -454,6 +454,9 @@
   </si>
   <si>
     <t>SCL</t>
+  </si>
+  <si>
+    <t>Hall effect sensor</t>
   </si>
 </sst>
 </file>
@@ -993,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1474,12 +1477,12 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9" t="s">
-        <v>57</v>
+      <c r="A42" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1488,7 +1491,7 @@
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1497,7 +1500,7 @@
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1506,7 +1509,7 @@
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1515,7 +1518,7 @@
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1524,7 +1527,7 @@
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1533,7 +1536,7 @@
       </c>
       <c r="B48" s="9"/>
       <c r="C48" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1542,16 +1545,16 @@
       </c>
       <c r="B49" s="9"/>
       <c r="C49" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -1560,18 +1563,16 @@
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -1579,30 +1580,32 @@
         <v>67</v>
       </c>
       <c r="B53" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C54" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="16" t="s">
+    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B55" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="C55" s="16" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1611,6 +1614,15 @@
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1623,7 +1635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="150" workbookViewId="0">
+    <sheetView showRowColHeaders="0" topLeftCell="A47" zoomScale="150" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2558,7 +2570,7 @@
       </c>
       <c r="D62" t="str">
         <f>IF(ISNUMBER(MATCH("A6", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Free</v>
+        <v>Used</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update wiring diagram and pin table for new rear IR array
</commit_message>
<xml_diff>
--- a/Pins/Organized_Pin_Table.xlsx
+++ b/Pins/Organized_Pin_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kin\mechatronics-goats\Pins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17743136-FBA6-4DC2-801E-FBC7F84BE220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543EE64F-9962-4CF2-B431-54AB06BDF95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-6855" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="143">
   <si>
     <t>Hardware Device</t>
   </si>
@@ -460,13 +460,16 @@
   </si>
   <si>
     <t>A99</t>
+  </si>
+  <si>
+    <t>IR Array 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,6 +508,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -999,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,7 +1638,62 @@
         <v>74</v>
       </c>
     </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2603,7 +2667,7 @@
       </c>
       <c r="D64" t="str">
         <f>IF(ISNUMBER(MATCH("A8", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Free</v>
+        <v>Used</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2618,7 +2682,7 @@
       </c>
       <c r="D65" t="str">
         <f>IF(ISNUMBER(MATCH("A9", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Free</v>
+        <v>Used</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2633,7 +2697,7 @@
       </c>
       <c r="D66" t="str">
         <f>IF(ISNUMBER(MATCH("A10", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Free</v>
+        <v>Used</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2648,7 +2712,7 @@
       </c>
       <c r="D67" t="str">
         <f>IF(ISNUMBER(MATCH("A11", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Free</v>
+        <v>Used</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2663,7 +2727,7 @@
       </c>
       <c r="D68" t="str">
         <f>IF(ISNUMBER(MATCH("A12", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Free</v>
+        <v>Used</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2678,7 +2742,7 @@
       </c>
       <c r="D69" t="str">
         <f>IF(ISNUMBER(MATCH("A13", Usages!$C:$C, 0)), "Used", "Free")</f>
-        <v>Free</v>
+        <v>Used</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>